<commit_message>
Maj liste des exigences
</commit_message>
<xml_diff>
--- a/modelisator/Gestion de projet/2015_05_28 [Modelisator] Step 2/2015_05_28 [Modelisator] Liste des exigences.xlsx
+++ b/modelisator/Gestion de projet/2015_05_28 [Modelisator] Step 2/2015_05_28 [Modelisator] Liste des exigences.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Type</t>
   </si>
@@ -51,12 +49,6 @@
     <t>Documentation suffisante pour un développeur logiciel</t>
   </si>
   <si>
-    <t>Pouvoir saisir un paramètre</t>
-  </si>
-  <si>
-    <t>Pouvoir saisir un objet physique</t>
-  </si>
-  <si>
     <t>Objet physique</t>
   </si>
   <si>
@@ -85,6 +77,48 @@
   </si>
   <si>
     <t>+/- 10% minutes</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>Grandeur physique</t>
+  </si>
+  <si>
+    <t>Visualiser toutes les GP liées directement à une GP</t>
+  </si>
+  <si>
+    <t>Graphe des GP</t>
+  </si>
+  <si>
+    <t>Calculer une GP à partir d'autres GP</t>
+  </si>
+  <si>
+    <t>Résultats de calculs mathématiques</t>
+  </si>
+  <si>
+    <t>Pouvoir modéliser un objet physique en fonction de ses GP</t>
+  </si>
+  <si>
+    <t>Toutes les GP du contexte modélisables</t>
+  </si>
+  <si>
+    <t>Pouvoir renseigner une valeur de GP non calculée</t>
+  </si>
+  <si>
+    <t>Toutes les valeurs saisies sont modifiables</t>
+  </si>
+  <si>
+    <t>Toutes les GP calculables depuis les GP saisies</t>
+  </si>
+  <si>
+    <t>Minimum 2 OS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Système d'exploitation (Operating System)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -299,35 +333,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -389,11 +399,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -419,9 +466,6 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -455,9 +499,30 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -467,49 +532,37 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -816,24 +869,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="17" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="11" width="9.140625" style="35"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -841,25 +896,21 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -877,287 +928,248 @@
         <v>6</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="11"/>
+      <c r="C4" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="32" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="E10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="F11" s="41"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
+      <c r="B14" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="16"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="16"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="16"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="15"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
@@ -1165,23 +1177,17 @@
       <c r="E24" s="1"/>
       <c r="F24" s="15"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="15"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
@@ -1189,195 +1195,133 @@
       <c r="E26" s="1"/>
       <c r="F26" s="16"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="17"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="17"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="17"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="17"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="17"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="17"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="17"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="17"/>
+      <c r="F35" s="16"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="17"/>
+      <c r="F36" s="16"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="17"/>
+      <c r="F37" s="16"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="F40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F45" s="19"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F46" s="19"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B14:B17"/>
     <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1405,34 +1349,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F19:F22 F4:F17</xm:sqref>
+          <xm:sqref>F17:F20 F4:F15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Maj fin de journée du 28/05/2015
</commit_message>
<xml_diff>
--- a/modelisator/Gestion de projet/2015_05_28 [Modelisator] Step 2/2015_05_28 [Modelisator] Liste des exigences.xlsx
+++ b/modelisator/Gestion de projet/2015_05_28 [Modelisator] Step 2/2015_05_28 [Modelisator] Liste des exigences.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Type</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Système d'exploitation (Operating System)</t>
+  </si>
+  <si>
+    <t>Performance de l'application</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -436,11 +439,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -511,9 +556,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -523,24 +565,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -550,12 +574,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -564,6 +582,48 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +944,7 @@
     <col min="5" max="5" width="13.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="11" width="9.140625" style="35"/>
+    <col min="8" max="11" width="9.140625" style="28"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -899,16 +959,16 @@
     </row>
     <row r="2" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -931,16 +991,16 @@
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="40" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="8"/>
@@ -948,8 +1008,8 @@
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="41" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -963,8 +1023,8 @@
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="41" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="21" t="s">
@@ -978,8 +1038,8 @@
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="41" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -993,8 +1053,8 @@
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -1008,7 +1068,7 @@
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="32"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1018,80 +1078,82 @@
       <c r="E9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E12" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="34" t="s">
-        <v>33</v>
+      <c r="B14" s="27" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -1099,11 +1161,11 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1112,7 +1174,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1148,7 +1210,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="14"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1175,7 +1237,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1184,7 +1246,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="16"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,9 +1359,15 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="F38" s="18"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
       <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1316,12 +1384,15 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1329,7 +1400,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{5AC6BB7E-4C8C-49D9-85E7-5825BB96D643}">
+          <x14:cfRule type="iconSet" priority="2" id="{5AC6BB7E-4C8C-49D9-85E7-5825BB96D643}">
             <x14:iconSet iconSet="4TrafficLights" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1349,7 +1420,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F17:F20 F4:F15</xm:sqref>
+          <xm:sqref>F18:F21 F11:F16 F4:F9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>